<commit_message>
refactored and fixed issues, unit test passes now
</commit_message>
<xml_diff>
--- a/tests/assets/PlfaToolAggregator_exampleTransformations.xlsx
+++ b/tests/assets/PlfaToolAggregator_exampleTransformations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brcarlson\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Projects\CafLogisticsPlfaToolsAggregator\plfa_tools_aggregator\tests\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41845EB-3C82-4EFC-862B-125D7C1A15E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0BB683D-5DD7-466D-9DDC-C4EDEC8750D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="1500" windowWidth="16788" windowHeight="21600" activeTab="2" xr2:uid="{FB7A8F59-C70E-4C47-A9DF-5FA134CD812A}"/>
+    <workbookView xWindow="-25920" yWindow="4044" windowWidth="25572" windowHeight="18756" activeTab="2" xr2:uid="{FB7A8F59-C70E-4C47-A9DF-5FA134CD812A}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="2" r:id="rId1"/>
@@ -35,21 +35,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
-    <t>SampleId</t>
-  </si>
-  <si>
-    <t>GCRunId</t>
-  </si>
-  <si>
     <t>GCFileLoc</t>
   </si>
   <si>
     <t>ProcessingCode</t>
   </si>
   <si>
-    <t>ProcessMethod</t>
-  </si>
-  <si>
     <t>RunDateTime</t>
   </si>
   <si>
@@ -150,6 +141,15 @@
   </si>
   <si>
     <t>Protozoa</t>
+  </si>
+  <si>
+    <t>SampleID</t>
+  </si>
+  <si>
+    <t>GCRunID</t>
+  </si>
+  <si>
+    <t>ProcessingMethod</t>
   </si>
 </sst>
 </file>
@@ -579,10 +579,10 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="G1" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -595,7 +595,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B3" s="7">
         <v>10001</v>
@@ -609,18 +609,18 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B4" s="7">
         <v>0</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E4" s="6"/>
       <c r="G4" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H4" s="9">
         <v>43699.766192129631</v>
@@ -636,31 +636,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="F6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="G6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="H6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="I6" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -680,13 +680,13 @@
         <v>2</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I7" s="5"/>
     </row>
@@ -707,13 +707,13 @@
         <v>4</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G8" s="4">
         <v>21.245850448486884</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I8" s="5"/>
     </row>
@@ -734,13 +734,13 @@
         <v>6</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G9" s="4">
         <v>4.5850209133993554</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I9" s="5"/>
     </row>
@@ -761,13 +761,13 @@
         <v>7</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G10" s="4">
         <v>55.881728633820615</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I10" s="5"/>
     </row>
@@ -788,13 +788,13 @@
         <v>8</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G11" s="4">
         <v>16.996550862982744</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I11" s="5"/>
     </row>
@@ -815,13 +815,13 @@
         <v>9</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G12" s="4">
         <v>1.2908491413103871</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I12" s="5"/>
     </row>
@@ -835,7 +835,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7">
@@ -844,7 +844,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G14" s="7">
         <v>24949.746252554462</v>
@@ -852,7 +852,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="8">
@@ -861,7 +861,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G15" s="7">
         <v>24949.746252554462</v>
@@ -879,13 +879,13 @@
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="18"/>
@@ -910,7 +910,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,22 +934,22 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
       <c r="G1" t="str">
         <f>raw!A6</f>
@@ -1346,7 +1346,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1368,52 +1368,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" t="s">
         <v>35</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>